<commit_message>
First run of pipeline.
</commit_message>
<xml_diff>
--- a/data/Iron_Steel_data_US_2011_2001.xlsx
+++ b/data/Iron_Steel_data_US_2011_2001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LongRunDatabase/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FCF549-FAB6-DB42-AE8B-4731CF010107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897712FF-89D2-6F48-9EBD-81B71CF7ACE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25420" windowHeight="18880" xr2:uid="{AEB495B6-756E-49E3-B271-872A24D79180}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="92">
   <si>
     <t>Country</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>Electric arc furnaces</t>
+  </si>
+  <si>
+    <t>Resources [of Wind]</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1150,7 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1191,7 +1194,7 @@
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
@@ -1214,7 +1217,7 @@
         <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -1237,7 +1240,7 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -1260,7 +1263,7 @@
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
@@ -1283,7 +1286,7 @@
         <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -1306,7 +1309,7 @@
         <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -1329,7 +1332,7 @@
         <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
         <v>47</v>
@@ -1352,7 +1355,7 @@
         <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
@@ -1375,7 +1378,7 @@
         <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
         <v>47</v>
@@ -1395,10 +1398,10 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Updated for Ricardo's latest data.
</commit_message>
<xml_diff>
--- a/data/Iron_Steel_data_US_2011_2001.xlsx
+++ b/data/Iron_Steel_data_US_2011_2001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LongRunDatabase/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7337B39F-9D7C-FE46-B6A5-E54056F27F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B55F00-D55D-694A-9FDF-A42BE405C9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25420" windowHeight="18880" xr2:uid="{AEB495B6-756E-49E3-B271-872A24D79180}"/>
+    <workbookView xWindow="22160" yWindow="500" windowWidth="29040" windowHeight="16440" xr2:uid="{AEB495B6-756E-49E3-B271-872A24D79180}"/>
   </bookViews>
   <sheets>
     <sheet name="Iron and steel" sheetId="3" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="69">
   <si>
     <t>Country</t>
   </si>
@@ -59,7 +48,16 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Computers</t>
+    <t>Iron and Steel</t>
+  </si>
+  <si>
+    <t>Room_air_conditioners</t>
+  </si>
+  <si>
+    <t>Commercial_indoor_electric_lamps</t>
+  </si>
+  <si>
+    <t>Electric_arc_furnaces</t>
   </si>
   <si>
     <t>LTC.20.C</t>
@@ -77,6 +75,9 @@
     <t>IP</t>
   </si>
   <si>
+    <t>Electronics (if no more detail)</t>
+  </si>
+  <si>
     <t>Main activity producer electricity plants</t>
   </si>
   <si>
@@ -86,6 +87,9 @@
     <t>Losses</t>
   </si>
   <si>
+    <t>Coal &amp; coal products (if no detail)</t>
+  </si>
+  <si>
     <t>Natural gas</t>
   </si>
   <si>
@@ -101,30 +105,18 @@
     <t>Solar thermal</t>
   </si>
   <si>
+    <t>Oil &amp; oil products (if no detail)</t>
+  </si>
+  <si>
     <t>Non-specified primary biofuels and waste</t>
   </si>
   <si>
-    <t>Gross final electricity</t>
-  </si>
-  <si>
-    <t>Final electricity</t>
-  </si>
-  <si>
-    <t>Energy Industry own use</t>
-  </si>
-  <si>
     <t>TJ</t>
   </si>
   <si>
     <t>USA</t>
   </si>
   <si>
-    <t>Coal mines</t>
-  </si>
-  <si>
-    <t>Oil and gas extraction</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -143,49 +135,37 @@
     <t>Gas extraction</t>
   </si>
   <si>
-    <t>Hydro - Dam</t>
-  </si>
-  <si>
-    <t>Nuclear - Plant</t>
-  </si>
-  <si>
-    <t>Geothermal - Plant</t>
-  </si>
-  <si>
-    <t>Solar photovoltaics - Plant</t>
-  </si>
-  <si>
-    <t>Solar thermal - Plant</t>
-  </si>
-  <si>
-    <t>Wind - Turbine</t>
-  </si>
-  <si>
-    <t>Non-specified primary biofuels and waste - Plant</t>
+    <t>Resources [of Wind]</t>
+  </si>
+  <si>
+    <t>Resources [of Geothermal]</t>
+  </si>
+  <si>
+    <t>Resources [of Solar PV]</t>
+  </si>
+  <si>
+    <t>Resources [of Solar Thermal]</t>
+  </si>
+  <si>
+    <t>Resources [of Hydro]</t>
+  </si>
+  <si>
+    <t>Resources [of Nuclear]</t>
+  </si>
+  <si>
+    <t>Resources [of Biofuels]</t>
+  </si>
+  <si>
+    <t>Resources [of Natural Gas]</t>
+  </si>
+  <si>
+    <t>Resources [of Crude Oil]</t>
   </si>
   <si>
     <t>Resources [of Coal]</t>
   </si>
   <si>
-    <t>Resources [of Natural Gas]</t>
-  </si>
-  <si>
-    <t>Resources [of Biofuels]</t>
-  </si>
-  <si>
-    <t>Resources [of Nuclear]</t>
-  </si>
-  <si>
-    <t>Resources [of Hydro]</t>
-  </si>
-  <si>
-    <t>Resources [of Geothermal]</t>
-  </si>
-  <si>
-    <t>Resources [of Solar PV]</t>
-  </si>
-  <si>
-    <t>Resources [of Solar Thermal]</t>
+    <t>Coal &amp; Coal products [from Resources]</t>
   </si>
   <si>
     <t>Oil &amp; oil products [from Resources]</t>
@@ -206,7 +186,7 @@
     <t>Geothermal [from Resources]</t>
   </si>
   <si>
-    <t>Solar photovoltaics [from Resources]</t>
+    <t>Solar PV [from Resources]</t>
   </si>
   <si>
     <t>Solar thermal [from Resources]</t>
@@ -215,49 +195,43 @@
     <t>Wind [from Resources]</t>
   </si>
   <si>
-    <t>Commercial indoor electric lamps</t>
-  </si>
-  <si>
-    <t>Room air conditioners</t>
-  </si>
-  <si>
-    <t>Electric arc furnaces</t>
-  </si>
-  <si>
-    <t>Resources [of Wind]</t>
-  </si>
-  <si>
-    <t>Iron and steel</t>
+    <t xml:space="preserve">Coal mines </t>
+  </si>
+  <si>
+    <t>Manufacture [of Non-specified primary biofuels and waste]</t>
+  </si>
+  <si>
+    <t>Manufacture [of Nuclear]</t>
+  </si>
+  <si>
+    <t>Manufacture [of Hydro]</t>
+  </si>
+  <si>
+    <t>Manufacture [of Geothermal]</t>
+  </si>
+  <si>
+    <t>Manufacture [of Solar PV]</t>
+  </si>
+  <si>
+    <t>Manufacture [of Solar thermal]</t>
+  </si>
+  <si>
+    <t>Manufacture [of Wind]</t>
+  </si>
+  <si>
+    <t>Nuclear industry</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Televisions</t>
   </si>
   <si>
     <t>Energy.type</t>
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>Resources [of Crude oil]</t>
-  </si>
-  <si>
-    <t>Resources [of Oil &amp; oil products]</t>
-  </si>
-  <si>
-    <t>Resources [of Coal &amp; coal products]</t>
-  </si>
-  <si>
-    <t>Coal &amp; coal products [from Resources]</t>
-  </si>
-  <si>
-    <t>Coal &amp; coal products</t>
-  </si>
-  <si>
-    <t>Oil &amp; oil products</t>
-  </si>
-  <si>
-    <t>Resources [of Solar thermal]</t>
-  </si>
-  <si>
-    <t>Electronics (if no detail)</t>
   </si>
 </sst>
 </file>
@@ -734,8 +708,9 @@
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1 2" xfId="20" xr:uid="{BA3FAA8D-0223-4495-B0F2-D431570AFFB8}"/>
@@ -1093,21 +1068,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E5F62F-9A49-4CB7-A026-5E77B3A048B6}">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="5" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="24.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1115,10 +1088,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1141,22 +1114,22 @@
         <v>2001</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>472747.88519266987</v>
@@ -1167,22 +1140,22 @@
         <v>2001</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>27006.850551094252</v>
@@ -1193,22 +1166,22 @@
         <v>2001</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H4">
         <v>94116.480115548373</v>
@@ -1219,22 +1192,22 @@
         <v>2001</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H5">
         <v>8735.5658465153338</v>
@@ -1245,22 +1218,22 @@
         <v>2001</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H6">
         <v>201578.96804885281</v>
@@ -1271,22 +1244,22 @@
         <v>2001</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H7">
         <v>15526.705712638632</v>
@@ -1297,22 +1270,22 @@
         <v>2001</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H8">
         <v>12025.093717141597</v>
@@ -1323,22 +1296,22 @@
         <v>2001</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H9">
         <v>0.25182701545615738</v>
@@ -1349,22 +1322,22 @@
         <v>2001</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H10">
         <v>139.45906815325068</v>
@@ -1375,22 +1348,22 @@
         <v>2001</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H11">
         <v>571.20877517057625</v>
@@ -1401,22 +1374,22 @@
         <v>2001</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H12">
         <v>472747.88519266987</v>
@@ -1427,22 +1400,22 @@
         <v>2001</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H13">
         <v>27006.850551094252</v>
@@ -1453,22 +1426,22 @@
         <v>2001</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H14">
         <v>94116.480115548373</v>
@@ -1479,22 +1452,22 @@
         <v>2001</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H15">
         <v>8735.5658465153338</v>
@@ -1505,22 +1478,22 @@
         <v>2001</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H16">
         <v>201578.96804885281</v>
@@ -1531,22 +1504,22 @@
         <v>2001</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H17">
         <v>15526.705712638632</v>
@@ -1557,22 +1530,22 @@
         <v>2001</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H18">
         <v>12025.093717141597</v>
@@ -1583,22 +1556,22 @@
         <v>2001</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H19">
         <v>0.25182701545615738</v>
@@ -1609,22 +1582,22 @@
         <v>2001</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H20">
         <v>139.45906815325068</v>
@@ -1635,22 +1608,22 @@
         <v>2001</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H21">
         <v>571.20877517057625</v>
@@ -1661,22 +1634,22 @@
         <v>2001</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H22">
         <v>472747.88519266987</v>
@@ -1687,22 +1660,22 @@
         <v>2001</v>
       </c>
       <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
         <v>26</v>
       </c>
-      <c r="C23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" t="s">
-        <v>71</v>
-      </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H23">
         <v>27006.850551094252</v>
@@ -1713,22 +1686,22 @@
         <v>2001</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H24">
         <v>94116.480115548373</v>
@@ -1739,22 +1712,22 @@
         <v>2001</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G25" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H25">
         <v>8735.5658465153338</v>
@@ -1765,22 +1738,22 @@
         <v>2001</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H26">
         <v>201578.96804885281</v>
@@ -1791,22 +1764,22 @@
         <v>2001</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H27">
         <v>15526.705712638632</v>
@@ -1817,22 +1790,22 @@
         <v>2001</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H28">
         <v>12025.093717141597</v>
@@ -1843,22 +1816,22 @@
         <v>2001</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H29">
         <v>0.25182701545615738</v>
@@ -1869,22 +1842,22 @@
         <v>2001</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H30">
         <v>139.45906815325068</v>
@@ -1895,22 +1868,22 @@
         <v>2001</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G31" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H31">
         <v>571.20877517057625</v>
@@ -1921,22 +1894,22 @@
         <v>2001</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G32" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H32">
         <v>472747.88519266987</v>
@@ -1947,22 +1920,22 @@
         <v>2001</v>
       </c>
       <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
         <v>26</v>
       </c>
-      <c r="C33" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" t="s">
-        <v>71</v>
-      </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G33" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H33">
         <v>27006.850551094252</v>
@@ -1973,22 +1946,22 @@
         <v>2001</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G34" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H34">
         <v>94116.480115548373</v>
@@ -1999,22 +1972,22 @@
         <v>2001</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G35" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H35">
         <v>8735.5658465153338</v>
@@ -2025,22 +1998,22 @@
         <v>2001</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="F36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G36" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H36">
         <v>201578.96804885281</v>
@@ -2051,22 +2024,22 @@
         <v>2001</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G37" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H37">
         <v>15526.705712638632</v>
@@ -2077,22 +2050,22 @@
         <v>2001</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F38" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G38" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H38">
         <v>12025.093717141597</v>
@@ -2103,22 +2076,22 @@
         <v>2001</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D39" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F39" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G39" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H39">
         <v>0.25182701545615738</v>
@@ -2129,22 +2102,22 @@
         <v>2001</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G40" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H40">
         <v>139.45906815325068</v>
@@ -2155,22 +2128,22 @@
         <v>2001</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G41" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H41">
         <v>571.20877517057625</v>
@@ -2181,25 +2154,25 @@
         <v>2001</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
         <v>65</v>
       </c>
-      <c r="D42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" t="s">
-        <v>22</v>
-      </c>
       <c r="F42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G42" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H42">
-        <v>293702.08801868692</v>
+        <v>227181.02855651936</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -2207,25 +2180,25 @@
         <v>2001</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" t="s">
         <v>65</v>
-      </c>
-      <c r="D43" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" t="s">
-        <v>24</v>
       </c>
       <c r="F43" t="s">
         <v>32</v>
       </c>
       <c r="G43" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H43">
-        <v>25142.580588175388</v>
+        <v>66521.059462167526</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -2233,25 +2206,25 @@
         <v>2001</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
         <v>65</v>
       </c>
-      <c r="D44" t="s">
-        <v>22</v>
-      </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="F44" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G44" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H44">
-        <v>268559.50743051153</v>
+        <v>2519.2197440225759</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2259,25 +2232,25 @@
         <v>2001</v>
       </c>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" t="s">
         <v>65</v>
       </c>
-      <c r="D45" t="s">
-        <v>15</v>
-      </c>
       <c r="E45" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F45" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G45" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H45">
-        <v>243169.20164880005</v>
+        <v>5811.7611381500055</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -2285,25 +2258,25 @@
         <v>2001</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s">
         <v>65</v>
       </c>
-      <c r="D46" t="s">
-        <v>23</v>
-      </c>
       <c r="E46" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="F46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G46" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H46">
-        <v>16213.295816770667</v>
+        <v>1062.1084802901846</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2311,25 +2284,25 @@
         <v>2001</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" t="s">
         <v>65</v>
       </c>
-      <c r="D47" t="s">
-        <v>23</v>
-      </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F47" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G47" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H47">
-        <v>20842.124690164681</v>
+        <v>562.01759224447733</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2337,25 +2310,25 @@
         <v>2001</v>
       </c>
       <c r="B48" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
         <v>65</v>
       </c>
-      <c r="D48" t="s">
-        <v>23</v>
-      </c>
       <c r="E48" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G48" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H48">
-        <v>202233.74899066074</v>
+        <v>15187.473633468149</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2363,25 +2336,25 @@
         <v>2001</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s">
         <v>65</v>
       </c>
-      <c r="D49" t="s">
-        <v>23</v>
-      </c>
       <c r="E49" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G49" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H49">
-        <v>3880.0321512039718</v>
+        <v>25390.305781711475</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2389,25 +2362,25 @@
         <v>2001</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" t="s">
         <v>65</v>
       </c>
-      <c r="D50" t="s">
-        <v>59</v>
-      </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F50" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G50" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H50">
-        <v>1633.5267299185612</v>
+        <v>16213.295816770667</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2415,25 +2388,25 @@
         <v>2001</v>
       </c>
       <c r="B51" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" t="s">
         <v>65</v>
-      </c>
-      <c r="D51" t="s">
-        <v>60</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G51" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H51">
-        <v>1055.8005643889253</v>
+        <v>20842.124690164681</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2441,25 +2414,25 @@
         <v>2001</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" t="s">
         <v>65</v>
-      </c>
-      <c r="D52" t="s">
-        <v>61</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G52" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H52">
-        <v>115554.74536149355</v>
+        <v>202233.74899066074</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2467,25 +2440,25 @@
         <v>2001</v>
       </c>
       <c r="B53" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" t="s">
         <v>65</v>
       </c>
-      <c r="D53" t="s">
-        <v>73</v>
-      </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G53" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H53">
-        <v>39.509909282668751</v>
+        <v>3880.0321512039718</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2493,25 +2466,25 @@
         <v>2001</v>
       </c>
       <c r="B54" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="F54" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G54" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H54">
-        <v>1633.5267299185607</v>
+        <v>1633.5267299185612</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2519,22 +2492,22 @@
         <v>2001</v>
       </c>
       <c r="B55" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C55" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D55" t="s">
         <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="F55" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G55" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H55">
         <v>1055.8005643889253</v>
@@ -2545,22 +2518,22 @@
         <v>2001</v>
       </c>
       <c r="B56" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D56" t="s">
         <v>10</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G56" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H56">
         <v>115554.74536149355</v>
@@ -2571,22 +2544,22 @@
         <v>2001</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C57" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E57" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F57" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G57" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H57">
         <v>39.509909282668751</v>
@@ -2594,106 +2567,106 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D58" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="E58" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="F58" t="s">
         <v>30</v>
       </c>
       <c r="G58" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H58">
-        <v>258721.20727663048</v>
+        <v>1633.5267299185607</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="E59" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F59" t="s">
         <v>30</v>
       </c>
       <c r="G59" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H59">
-        <v>3935.7033941519708</v>
+        <v>1055.8005643889253</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="B60" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D60" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="F60" t="s">
         <v>30</v>
       </c>
       <c r="G60" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H60">
-        <v>91096.792059987623</v>
+        <v>115554.74536149355</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="B61" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E61" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="F61" t="s">
         <v>30</v>
       </c>
       <c r="G61" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H61">
-        <v>7081.9471263613977</v>
+        <v>39.509909282668751</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2701,25 +2674,25 @@
         <v>2011</v>
       </c>
       <c r="B62" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D62" t="s">
         <v>45</v>
       </c>
       <c r="E62" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F62" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G62" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H62">
-        <v>130891.37607398616</v>
+        <v>258721.20727663048</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2727,25 +2700,25 @@
         <v>2011</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C63" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D63" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E63" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F63" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G63" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H63">
-        <v>16821.743673772831</v>
+        <v>3935.7033941519708</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2753,25 +2726,25 @@
         <v>2011</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D64" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E64" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F64" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G64" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H64">
-        <v>5082.0862382809401</v>
+        <v>91096.792059987623</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2779,25 +2752,25 @@
         <v>2011</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D65" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E65" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G65" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H65">
-        <v>49.167608688405451</v>
+        <v>7081.9471263613977</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2805,25 +2778,25 @@
         <v>2011</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D66" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E66" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G66" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H66">
-        <v>114.70986486764619</v>
+        <v>130891.37607398616</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2831,25 +2804,25 @@
         <v>2011</v>
       </c>
       <c r="B67" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="E67" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G67" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H67">
-        <v>6352.2469858662262</v>
+        <v>16821.743673772831</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2857,25 +2830,25 @@
         <v>2011</v>
       </c>
       <c r="B68" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C68" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D68" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="E68" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="F68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G68" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H68">
-        <v>258721.20727663048</v>
+        <v>5082.0862382809401</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2883,25 +2856,25 @@
         <v>2011</v>
       </c>
       <c r="B69" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D69" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E69" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F69" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G69" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H69">
-        <v>3935.7033941519708</v>
+        <v>49.167608688405451</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2909,25 +2882,25 @@
         <v>2011</v>
       </c>
       <c r="B70" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D70" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E70" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="F70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G70" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H70">
-        <v>91096.792059987623</v>
+        <v>114.70986486764619</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2935,25 +2908,25 @@
         <v>2011</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D71" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E71" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G71" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H71">
-        <v>7081.9471263613977</v>
+        <v>6352.2469858662262</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2961,25 +2934,25 @@
         <v>2011</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D72" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E72" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="F72" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G72" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H72">
-        <v>130891.37607398616</v>
+        <v>258721.20727663048</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2987,25 +2960,25 @@
         <v>2011</v>
       </c>
       <c r="B73" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D73" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F73" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G73" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H73">
-        <v>16821.743673772831</v>
+        <v>3935.7033941519708</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -3013,25 +2986,25 @@
         <v>2011</v>
       </c>
       <c r="B74" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D74" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E74" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F74" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G74" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H74">
-        <v>5082.0862382809401</v>
+        <v>91096.792059987623</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -3039,25 +3012,25 @@
         <v>2011</v>
       </c>
       <c r="B75" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C75" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D75" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E75" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="F75" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G75" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H75">
-        <v>49.167608688405451</v>
+        <v>7081.9471263613977</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -3065,25 +3038,25 @@
         <v>2011</v>
       </c>
       <c r="B76" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C76" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D76" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E76" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F76" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G76" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H76">
-        <v>114.70986486764619</v>
+        <v>130891.37607398616</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -3091,25 +3064,25 @@
         <v>2011</v>
       </c>
       <c r="B77" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C77" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D77" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E77" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="F77" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G77" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H77">
-        <v>6352.2469858662262</v>
+        <v>16821.743673772831</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -3117,25 +3090,25 @@
         <v>2011</v>
       </c>
       <c r="B78" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C78" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D78" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E78" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F78" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G78" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H78">
-        <v>258721.20727663048</v>
+        <v>5082.0862382809401</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -3143,25 +3116,25 @@
         <v>2011</v>
       </c>
       <c r="B79" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D79" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="E79" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F79" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G79" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H79">
-        <v>3935.7033941519708</v>
+        <v>49.167608688405451</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -3169,25 +3142,25 @@
         <v>2011</v>
       </c>
       <c r="B80" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C80" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D80" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E80" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="F80" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G80" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H80">
-        <v>91096.792059987623</v>
+        <v>114.70986486764619</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -3195,25 +3168,25 @@
         <v>2011</v>
       </c>
       <c r="B81" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C81" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D81" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E81" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G81" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H81">
-        <v>7081.9471263613977</v>
+        <v>6352.2469858662262</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -3221,25 +3194,25 @@
         <v>2011</v>
       </c>
       <c r="B82" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D82" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E82" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G82" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H82">
-        <v>130891.37607398616</v>
+        <v>258721.20727663048</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -3247,25 +3220,25 @@
         <v>2011</v>
       </c>
       <c r="B83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" t="s">
         <v>26</v>
       </c>
-      <c r="C83" t="s">
-        <v>65</v>
-      </c>
-      <c r="D83" t="s">
-        <v>35</v>
-      </c>
-      <c r="E83" t="s">
-        <v>9</v>
-      </c>
       <c r="F83" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G83" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H83">
-        <v>16821.743673772831</v>
+        <v>3935.7033941519708</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -3273,25 +3246,25 @@
         <v>2011</v>
       </c>
       <c r="B84" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C84" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D84" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E84" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F84" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G84" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H84">
-        <v>5082.0862382809401</v>
+        <v>91096.792059987623</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -3299,25 +3272,25 @@
         <v>2011</v>
       </c>
       <c r="B85" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C85" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D85" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E85" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F85" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G85" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H85">
-        <v>49.167608688405451</v>
+        <v>7081.9471263613977</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -3325,25 +3298,25 @@
         <v>2011</v>
       </c>
       <c r="B86" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C86" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D86" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E86" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F86" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G86" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H86">
-        <v>114.70986486764619</v>
+        <v>130891.37607398616</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -3351,25 +3324,25 @@
         <v>2011</v>
       </c>
       <c r="B87" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C87" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D87" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E87" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F87" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G87" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H87">
-        <v>6352.2469858662262</v>
+        <v>16821.743673772831</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -3377,25 +3350,25 @@
         <v>2011</v>
       </c>
       <c r="B88" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C88" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D88" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E88" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F88" t="s">
         <v>32</v>
       </c>
       <c r="G88" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H88">
-        <v>258721.20727663048</v>
+        <v>5082.0862382809401</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -3403,25 +3376,25 @@
         <v>2011</v>
       </c>
       <c r="B89" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C89" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D89" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E89" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F89" t="s">
         <v>32</v>
       </c>
       <c r="G89" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H89">
-        <v>3935.7033941519708</v>
+        <v>49.167608688405451</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -3429,25 +3402,25 @@
         <v>2011</v>
       </c>
       <c r="B90" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C90" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="E90" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F90" t="s">
         <v>32</v>
       </c>
       <c r="G90" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H90">
-        <v>91096.792059987623</v>
+        <v>114.70986486764619</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -3455,25 +3428,25 @@
         <v>2011</v>
       </c>
       <c r="B91" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C91" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D91" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E91" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F91" t="s">
         <v>32</v>
       </c>
       <c r="G91" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H91">
-        <v>7081.9471263613977</v>
+        <v>6352.2469858662262</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -3481,25 +3454,25 @@
         <v>2011</v>
       </c>
       <c r="B92" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C92" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D92" t="s">
+        <v>20</v>
+      </c>
+      <c r="E92" t="s">
         <v>17</v>
       </c>
-      <c r="E92" t="s">
-        <v>13</v>
-      </c>
       <c r="F92" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G92" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H92">
-        <v>130891.37607398616</v>
+        <v>258721.20727663048</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -3507,25 +3480,25 @@
         <v>2011</v>
       </c>
       <c r="B93" t="s">
+        <v>68</v>
+      </c>
+      <c r="C93" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93" t="s">
         <v>26</v>
       </c>
-      <c r="C93" t="s">
-        <v>65</v>
-      </c>
-      <c r="D93" t="s">
-        <v>9</v>
-      </c>
       <c r="E93" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F93" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G93" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H93">
-        <v>16821.743673772831</v>
+        <v>3935.7033941519708</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -3533,25 +3506,25 @@
         <v>2011</v>
       </c>
       <c r="B94" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C94" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D94" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E94" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F94" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G94" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H94">
-        <v>5082.0862382809401</v>
+        <v>91096.792059987623</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -3559,25 +3532,25 @@
         <v>2011</v>
       </c>
       <c r="B95" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C95" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D95" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E95" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F95" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G95" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H95">
-        <v>49.167608688405451</v>
+        <v>7081.9471263613977</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -3585,25 +3558,25 @@
         <v>2011</v>
       </c>
       <c r="B96" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C96" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D96" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E96" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="F96" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G96" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H96">
-        <v>114.70986486764619</v>
+        <v>130891.37607398616</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -3611,25 +3584,25 @@
         <v>2011</v>
       </c>
       <c r="B97" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C97" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D97" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E97" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F97" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G97" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H97">
-        <v>6352.2469858662262</v>
+        <v>16821.743673772831</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -3637,25 +3610,25 @@
         <v>2011</v>
       </c>
       <c r="B98" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C98" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D98" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E98" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F98" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G98" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H98">
-        <v>210299.60554318657</v>
+        <v>5082.0862382809401</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3663,25 +3636,25 @@
         <v>2011</v>
       </c>
       <c r="B99" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C99" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D99" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E99" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F99" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G99" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H99">
-        <v>210299.60554318657</v>
+        <v>49.167608688405451</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3689,25 +3662,25 @@
         <v>2011</v>
       </c>
       <c r="B100" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C100" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D100" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E100" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F100" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G100" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H100">
-        <v>174913.19963999998</v>
+        <v>114.70986486764619</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -3715,25 +3688,25 @@
         <v>2011</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C101" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D101" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E101" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="F101" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G101" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H101">
-        <v>12338.623209035801</v>
+        <v>6352.2469858662262</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -3741,25 +3714,25 @@
         <v>2011</v>
       </c>
       <c r="B102" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C102" t="s">
+        <v>29</v>
+      </c>
+      <c r="D102" t="s">
+        <v>17</v>
+      </c>
+      <c r="E102" t="s">
         <v>65</v>
-      </c>
-      <c r="D102" t="s">
-        <v>23</v>
-      </c>
-      <c r="E102" t="s">
-        <v>60</v>
       </c>
       <c r="F102" t="s">
         <v>32</v>
       </c>
       <c r="G102" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H102">
-        <v>17277.248655626187</v>
+        <v>167105.45144185887</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -3767,25 +3740,25 @@
         <v>2011</v>
       </c>
       <c r="B103" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C103" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103" t="s">
+        <v>64</v>
+      </c>
+      <c r="E103" t="s">
         <v>65</v>
-      </c>
-      <c r="D103" t="s">
-        <v>23</v>
-      </c>
-      <c r="E103" t="s">
-        <v>61</v>
       </c>
       <c r="F103" t="s">
         <v>32</v>
       </c>
       <c r="G103" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H103">
-        <v>142294.95496406424</v>
+        <v>43194.154101327586</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -3793,25 +3766,25 @@
         <v>2011</v>
       </c>
       <c r="B104" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C104" t="s">
+        <v>29</v>
+      </c>
+      <c r="D104" t="s">
         <v>65</v>
       </c>
-      <c r="D104" t="s">
-        <v>23</v>
-      </c>
       <c r="E104" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="F104" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G104" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H104">
-        <v>3002.3728112737513</v>
+        <v>1596.8316075484458</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -3819,25 +3792,25 @@
         <v>2011</v>
       </c>
       <c r="B105" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C105" t="s">
+        <v>29</v>
+      </c>
+      <c r="D105" t="s">
         <v>65</v>
       </c>
-      <c r="D105" t="s">
-        <v>59</v>
-      </c>
       <c r="E105" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F105" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G105" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H105">
-        <v>1423.4838439907276</v>
+        <v>3704.8765525013209</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -3845,25 +3818,25 @@
         <v>2011</v>
       </c>
       <c r="B106" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C106" t="s">
+        <v>29</v>
+      </c>
+      <c r="D106" t="s">
         <v>65</v>
       </c>
-      <c r="D106" t="s">
-        <v>60</v>
-      </c>
       <c r="E106" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="F106" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G106" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H106">
-        <v>1085.8851527215943</v>
+        <v>840.89991731268697</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -3871,25 +3844,25 @@
         <v>2011</v>
       </c>
       <c r="B107" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C107" t="s">
+        <v>29</v>
+      </c>
+      <c r="D107" t="s">
         <v>65</v>
       </c>
-      <c r="D107" t="s">
-        <v>61</v>
-      </c>
       <c r="E107" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="F107" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G107" t="s">
-        <v>25</v>
-      </c>
-      <c r="H107">
-        <v>81737.537237089593</v>
+        <v>28</v>
+      </c>
+      <c r="H107" s="1">
+        <v>276.33913096592511</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -3897,25 +3870,25 @@
         <v>2011</v>
       </c>
       <c r="B108" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C108" t="s">
+        <v>29</v>
+      </c>
+      <c r="D108" t="s">
         <v>65</v>
       </c>
-      <c r="D108" t="s">
-        <v>7</v>
-      </c>
       <c r="E108" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F108" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G108" t="s">
-        <v>25</v>
-      </c>
-      <c r="H108">
-        <v>51.836523280945023</v>
+        <v>28</v>
+      </c>
+      <c r="H108" s="1">
+        <v>11742.246909125983</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -3923,25 +3896,25 @@
         <v>2011</v>
       </c>
       <c r="B109" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C109" t="s">
+        <v>29</v>
+      </c>
+      <c r="D109" t="s">
         <v>65</v>
       </c>
-      <c r="D109" t="s">
-        <v>11</v>
-      </c>
       <c r="E109" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="F109" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G109" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H109">
-        <v>1423.4838439907276</v>
+        <v>17225.211785732216</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -3949,25 +3922,25 @@
         <v>2011</v>
       </c>
       <c r="B110" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C110" t="s">
+        <v>29</v>
+      </c>
+      <c r="D110" t="s">
         <v>65</v>
       </c>
-      <c r="D110" t="s">
-        <v>8</v>
-      </c>
       <c r="E110" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="F110" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G110" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H110">
-        <v>1085.8851527215943</v>
+        <v>12338.623209035801</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -3975,25 +3948,25 @@
         <v>2011</v>
       </c>
       <c r="B111" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C111" t="s">
+        <v>29</v>
+      </c>
+      <c r="D111" t="s">
         <v>65</v>
       </c>
-      <c r="D111" t="s">
-        <v>10</v>
-      </c>
       <c r="E111" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="F111" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G111" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H111">
-        <v>81737.537237089593</v>
+        <v>17277.248655626187</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -4001,29 +3974,262 @@
         <v>2011</v>
       </c>
       <c r="B112" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C112" t="s">
+        <v>29</v>
+      </c>
+      <c r="D112" t="s">
         <v>65</v>
       </c>
-      <c r="D112" t="s">
-        <v>12</v>
-      </c>
       <c r="E112" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="F112" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G112" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H112">
+        <v>142294.95496406424</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>2011</v>
+      </c>
+      <c r="B113" t="s">
+        <v>68</v>
+      </c>
+      <c r="C113" t="s">
+        <v>29</v>
+      </c>
+      <c r="D113" t="s">
+        <v>65</v>
+      </c>
+      <c r="E113" t="s">
+        <v>66</v>
+      </c>
+      <c r="F113" t="s">
+        <v>33</v>
+      </c>
+      <c r="G113" t="s">
+        <v>28</v>
+      </c>
+      <c r="H113">
+        <v>3002.3728112737513</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>2011</v>
+      </c>
+      <c r="B114" t="s">
+        <v>68</v>
+      </c>
+      <c r="C114" t="s">
+        <v>29</v>
+      </c>
+      <c r="D114" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114" t="s">
+        <v>32</v>
+      </c>
+      <c r="G114" t="s">
+        <v>28</v>
+      </c>
+      <c r="H114">
+        <v>1423.4838439907276</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>2011</v>
+      </c>
+      <c r="B115" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" t="s">
+        <v>29</v>
+      </c>
+      <c r="D115" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" t="s">
+        <v>32</v>
+      </c>
+      <c r="G115" t="s">
+        <v>28</v>
+      </c>
+      <c r="H115">
+        <v>1085.8851527215943</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>2011</v>
+      </c>
+      <c r="B116" t="s">
+        <v>68</v>
+      </c>
+      <c r="C116" t="s">
+        <v>29</v>
+      </c>
+      <c r="D116" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" t="s">
+        <v>13</v>
+      </c>
+      <c r="F116" t="s">
+        <v>32</v>
+      </c>
+      <c r="G116" t="s">
+        <v>28</v>
+      </c>
+      <c r="H116">
+        <v>81737.537237089593</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>2011</v>
+      </c>
+      <c r="B117" t="s">
+        <v>68</v>
+      </c>
+      <c r="C117" t="s">
+        <v>29</v>
+      </c>
+      <c r="D117" t="s">
+        <v>16</v>
+      </c>
+      <c r="E117" t="s">
+        <v>15</v>
+      </c>
+      <c r="F117" t="s">
+        <v>32</v>
+      </c>
+      <c r="G117" t="s">
+        <v>28</v>
+      </c>
+      <c r="H117">
+        <v>51.836523280945023</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>2011</v>
+      </c>
+      <c r="B118" t="s">
+        <v>68</v>
+      </c>
+      <c r="C118" t="s">
+        <v>29</v>
+      </c>
+      <c r="D118" t="s">
+        <v>14</v>
+      </c>
+      <c r="E118" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118" t="s">
+        <v>30</v>
+      </c>
+      <c r="G118" t="s">
+        <v>28</v>
+      </c>
+      <c r="H118">
+        <v>1423.4838439907276</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>2011</v>
+      </c>
+      <c r="B119" t="s">
+        <v>68</v>
+      </c>
+      <c r="C119" t="s">
+        <v>29</v>
+      </c>
+      <c r="D119" t="s">
+        <v>11</v>
+      </c>
+      <c r="E119" t="s">
+        <v>7</v>
+      </c>
+      <c r="F119" t="s">
+        <v>30</v>
+      </c>
+      <c r="G119" t="s">
+        <v>28</v>
+      </c>
+      <c r="H119">
+        <v>1085.8851527215943</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>2011</v>
+      </c>
+      <c r="B120" t="s">
+        <v>68</v>
+      </c>
+      <c r="C120" t="s">
+        <v>29</v>
+      </c>
+      <c r="D120" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" t="s">
+        <v>7</v>
+      </c>
+      <c r="F120" t="s">
+        <v>30</v>
+      </c>
+      <c r="G120" t="s">
+        <v>28</v>
+      </c>
+      <c r="H120">
+        <v>81737.537237089593</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>2011</v>
+      </c>
+      <c r="B121" t="s">
+        <v>68</v>
+      </c>
+      <c r="C121" t="s">
+        <v>29</v>
+      </c>
+      <c r="D121" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" t="s">
+        <v>7</v>
+      </c>
+      <c r="F121" t="s">
+        <v>30</v>
+      </c>
+      <c r="G121" t="s">
+        <v>28</v>
+      </c>
+      <c r="H121">
         <v>51.836523280945023</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>